<commit_message>
updated files with latest revisions
</commit_message>
<xml_diff>
--- a/Doc/XML-SS-Correspondences.xlsx
+++ b/Doc/XML-SS-Correspondences.xlsx
@@ -9,12 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="26160" yWindow="620" windowWidth="21780" windowHeight="27160" tabRatio="500" activeTab="1"/>
-    <workbookView xWindow="1040" yWindow="1680" windowWidth="21820" windowHeight="24500" tabRatio="500"/>
+    <workbookView xWindow="23340" yWindow="1060" windowWidth="24900" windowHeight="27300" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Movies" sheetId="1" r:id="rId1"/>
-    <sheet name="TV" sheetId="2" r:id="rId2"/>
+    <sheet name="TV (episode)" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -47,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="212">
   <si>
     <t>Avail</t>
   </si>
@@ -397,54 +396,6 @@
     <t>Avail/Asset/WorkType</t>
   </si>
   <si>
-    <t>Avail/Asset/Metadata/TitleInternalAlias
-Avail/Asset/EpisodeMetadata/TitleInternalAlias</t>
-  </si>
-  <si>
-    <t>Avail/Asset/Metadata/TitleDisplayUnlimited
-Avail/Asset/EpisodeMetadata/TitleDisplayUnlimited</t>
-  </si>
-  <si>
-    <t>Avail/Asset/Metadata/AltIdentifier/Identifier
-Avail/Asset/EpisodeMetadata/AltIdentifier/Identifier</t>
-  </si>
-  <si>
-    <t>Avail/Asset/Metadata/LocalizationOffering
-Avail/Asset/EpisodeMetadata/LocalizationOffering</t>
-  </si>
-  <si>
-    <t>Avail/Asset/Metadata/ReleaseDate
-Avail/Asset/EpisodeMetadata/ReleaseDate</t>
-  </si>
-  <si>
-    <t>Avail/Asset/Metadata/RunLength
-Avail/Asset/EpisodeMetadata/RunLength</t>
-  </si>
-  <si>
-    <t>Avail/Asset/Metadata/USACaptionsExemptionReason
-Avail/Asset/EpisodeMetadata/USACaptionsExemptionReason</t>
-  </si>
-  <si>
-    <t>Avail/Asset/Metadata/Ratings/Rating/System
-Avail/Asset/EpisodeMetadata/Ratings/Rating/System</t>
-  </si>
-  <si>
-    <t>Avail/Asset/Metadata/Ratings/Rating/Value
-Avail/Asset/EpisodeMetadata/Ratings/Rating/Value</t>
-  </si>
-  <si>
-    <t>Avail/Asset/Metadata/Ratings/Rating/Reason
-Avail/Asset/EpisodeMetadata/Ratings/Rating/Reason</t>
-  </si>
-  <si>
-    <t>Avail/Asset/Metadata/ReleaseHistory/Date
-Avail/Asset/EpisodeMetadata/ReleaseHistory/Date</t>
-  </si>
-  <si>
-    <t>Date + Avail/Asset/Metadata/ReleaseHistory/ReleaseType 'DVD'
-Date + Avail/Asset/EpisodeMetadata/ReleaseHistory/ReleaseType 'DVD'</t>
-  </si>
-  <si>
     <t>absence of USACaptionsExemptionReason</t>
   </si>
   <si>
@@ -686,6 +637,120 @@
   </si>
   <si>
     <t>@termName + Avail/Transaction/Term/Event</t>
+  </si>
+  <si>
+    <t>Avail/Asset/Metadata/TitleInternalAlias</t>
+  </si>
+  <si>
+    <t>Avail/Asset/Metadata/TitleDisplayUnlimited</t>
+  </si>
+  <si>
+    <t>Avail/Asset/Metadata/LocalizationOffering</t>
+  </si>
+  <si>
+    <t>Avail/Asset/Metadata/AltIdentifier/Identifier</t>
+  </si>
+  <si>
+    <t>Avail/Asset/Metadata/ReleaseDate</t>
+  </si>
+  <si>
+    <t>Avail/Asset/Metadata/ReleaseHistory/Date</t>
+  </si>
+  <si>
+    <t>Date + Avail/Asset/Metadata/ReleaseHistory/ReleaseType 'DVD'</t>
+  </si>
+  <si>
+    <t>Avail/Asset/Metadata/Ratings/Rating/System</t>
+  </si>
+  <si>
+    <t>Avail/Asset/Metadata/Ratings/Rating/Value</t>
+  </si>
+  <si>
+    <t>Avail/Asset/Metadata/Ratings/Rating/Reason</t>
+  </si>
+  <si>
+    <t>Avail/Asset/Metadata/RunLength</t>
+  </si>
+  <si>
+    <t>Avail/Asset/Metadata/USACaptionsExemptionReason</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/TitleInternalAlias</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/EpisodeNumber</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/SeasonMetadata/SeasonNumber</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/LocalizationOffering</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/SeasonMetadata/TitleInternalAlias</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/SeasonMetadata/TitleDisplayUnlimited</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/SeasonMetadata/NumberOfEpisodes</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/AltIdentifier</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/SeasonMetadata/AltIdentifier</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/SeasonMetadata/SeriesMetadata/TitleInternalAlias</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/SeasonMetadata/SeriesMetadata/TitleDisplayUnlimited</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/SeasonMetadata/SeriesMetadata/NumberOfSeasons</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/SeasonMetadata/SeriesMetadata/AltIdentifier</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/RunLength</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/USACaptionsExemptionReason</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/Ratings/Rating/System</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/Ratings/Rating/Value</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/Ratings/Rating/Reason</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/ReleaseHistory/Date</t>
+  </si>
+  <si>
+    <t>Date + Avail/Asset/EpisodeMetadata/ReleaseHistory/ReleaseType 'DVD'</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/ReleaseDate</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/EncodeID</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/EditEIDR-S</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/SeasonMetadata/SeriesMetadata/SeriesContentID</t>
+  </si>
+  <si>
+    <t>Avail/Asset/EpisodeMetadata/SeasonMetadata/SeasonContentID</t>
   </si>
 </sst>
 </file>
@@ -868,7 +933,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1029,6 +1094,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1312,9 +1383,6 @@
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="E27" sqref="E27"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="1">
-      <selection activeCell="E43" sqref="E43:E44"/>
-    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1340,7 +1408,7 @@
         <v>1</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>122</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="91" x14ac:dyDescent="0.2">
@@ -1358,7 +1426,7 @@
         <v>4</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="26" x14ac:dyDescent="0.2">
@@ -1376,7 +1444,7 @@
         <v>6</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
@@ -1415,7 +1483,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>14</v>
       </c>
@@ -1430,10 +1498,10 @@
         <v>15</v>
       </c>
       <c r="E6" s="31" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="26" x14ac:dyDescent="0.2">
       <c r="A7" s="9" t="s">
         <v>14</v>
       </c>
@@ -1448,7 +1516,7 @@
         <v>17</v>
       </c>
       <c r="E7" s="31" t="s">
-        <v>96</v>
+        <v>175</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="117" x14ac:dyDescent="0.2">
@@ -1466,7 +1534,7 @@
         <v>19</v>
       </c>
       <c r="E8" s="31" t="s">
-        <v>98</v>
+        <v>176</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
@@ -1484,7 +1552,7 @@
         <v>21</v>
       </c>
       <c r="E9" s="30" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1502,7 +1570,7 @@
         <v>23</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1520,7 +1588,7 @@
         <v>25</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1538,7 +1606,7 @@
         <v>27</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="39" x14ac:dyDescent="0.2">
@@ -1556,7 +1624,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="26" x14ac:dyDescent="0.2">
@@ -1574,7 +1642,7 @@
         <v>31</v>
       </c>
       <c r="E14" s="30" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -1592,7 +1660,7 @@
         <v>33</v>
       </c>
       <c r="E15" s="32" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1610,7 +1678,7 @@
         <v>35</v>
       </c>
       <c r="E16" s="30" t="s">
-        <v>119</v>
+        <v>107</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
@@ -1628,7 +1696,7 @@
         <v>37</v>
       </c>
       <c r="E17" s="30" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
@@ -1646,7 +1714,7 @@
         <v>39</v>
       </c>
       <c r="E18" s="33" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -1664,7 +1732,7 @@
         <v>41</v>
       </c>
       <c r="E19" s="30" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1682,7 +1750,7 @@
         <v>43</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
@@ -1700,7 +1768,7 @@
         <v>45</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
@@ -1718,7 +1786,7 @@
         <v>47</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>130</v>
+        <v>118</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1736,7 +1804,7 @@
         <v>49</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>132</v>
+        <v>120</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1754,7 +1822,7 @@
         <v>51</v>
       </c>
       <c r="E24" s="33" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="91" x14ac:dyDescent="0.2">
@@ -1772,7 +1840,7 @@
         <v>53</v>
       </c>
       <c r="E25" s="31" t="s">
-        <v>97</v>
+        <v>177</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="78" x14ac:dyDescent="0.2">
@@ -1790,7 +1858,7 @@
         <v>55</v>
       </c>
       <c r="E26" s="30" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:5" ht="52" x14ac:dyDescent="0.2">
@@ -1808,10 +1876,10 @@
         <v>57</v>
       </c>
       <c r="E27" s="33" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="32" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" ht="26" x14ac:dyDescent="0.2">
       <c r="A28" s="9" t="s">
         <v>14</v>
       </c>
@@ -1826,7 +1894,7 @@
         <v>59</v>
       </c>
       <c r="E28" s="31" t="s">
-        <v>99</v>
+        <v>178</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="39" x14ac:dyDescent="0.2">
@@ -1844,7 +1912,7 @@
         <v>61</v>
       </c>
       <c r="E29" s="31" t="s">
-        <v>105</v>
+        <v>179</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="39" x14ac:dyDescent="0.2">
@@ -1862,7 +1930,7 @@
         <v>63</v>
       </c>
       <c r="E30" s="31" t="s">
-        <v>106</v>
+        <v>180</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="39" x14ac:dyDescent="0.2">
@@ -1880,7 +1948,7 @@
         <v>65</v>
       </c>
       <c r="E31" s="30" t="s">
-        <v>120</v>
+        <v>108</v>
       </c>
     </row>
     <row r="32" spans="1:5" ht="39" x14ac:dyDescent="0.2">
@@ -1898,7 +1966,7 @@
         <v>67</v>
       </c>
       <c r="E32" s="31" t="s">
-        <v>102</v>
+        <v>181</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="37" customHeight="1" x14ac:dyDescent="0.2">
@@ -1916,7 +1984,7 @@
         <v>69</v>
       </c>
       <c r="E33" s="31" t="s">
-        <v>103</v>
+        <v>182</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="52" x14ac:dyDescent="0.2">
@@ -1934,7 +2002,7 @@
         <v>71</v>
       </c>
       <c r="E34" s="31" t="s">
-        <v>104</v>
+        <v>183</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -1952,7 +2020,7 @@
         <v>73</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -1970,7 +2038,7 @@
         <v>75</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>121</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -1988,7 +2056,7 @@
         <v>77</v>
       </c>
       <c r="E37" s="32" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="182" x14ac:dyDescent="0.2">
@@ -2006,7 +2074,7 @@
         <v>79</v>
       </c>
       <c r="E38" s="31" t="s">
-        <v>101</v>
+        <v>185</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -2024,7 +2092,7 @@
         <v>81</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="26" x14ac:dyDescent="0.2">
@@ -2042,7 +2110,7 @@
         <v>83</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="39" x14ac:dyDescent="0.2">
@@ -2060,10 +2128,10 @@
         <v>85</v>
       </c>
       <c r="E41" s="30" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" ht="32" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42" s="9" t="s">
         <v>14</v>
       </c>
@@ -2078,7 +2146,7 @@
         <v>87</v>
       </c>
       <c r="E42" s="31" t="s">
-        <v>100</v>
+        <v>184</v>
       </c>
     </row>
     <row r="43" spans="1:7" ht="91" x14ac:dyDescent="0.2">
@@ -2096,7 +2164,7 @@
         <v>89</v>
       </c>
       <c r="E43" s="30" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:7" ht="104" x14ac:dyDescent="0.2">
@@ -2114,7 +2182,7 @@
         <v>91</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>118</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -7450,12 +7518,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7463,10 +7530,11 @@
     <col min="2" max="2" width="7.1640625" customWidth="1"/>
     <col min="3" max="3" width="61.1640625" customWidth="1"/>
     <col min="4" max="4" width="26.33203125" style="56" customWidth="1"/>
-    <col min="5" max="5" width="62.33203125" customWidth="1"/>
+    <col min="5" max="5" width="74" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="58"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
@@ -7481,10 +7549,13 @@
         <v>1</v>
       </c>
       <c r="E1" s="30" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="91" x14ac:dyDescent="0.2">
+        <v>110</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="91" x14ac:dyDescent="0.2">
       <c r="A2" s="38" t="s">
         <v>3</v>
       </c>
@@ -7499,10 +7570,13 @@
         <v>4</v>
       </c>
       <c r="E2" s="30" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A3" s="38" t="s">
         <v>3</v>
       </c>
@@ -7517,10 +7591,13 @@
         <v>6</v>
       </c>
       <c r="E3" s="30" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+      <c r="F3" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
         <v>8</v>
       </c>
@@ -7529,7 +7606,7 @@
         <v>3</v>
       </c>
       <c r="C4" s="34" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="D4" s="49" t="s">
         <v>9</v>
@@ -7537,8 +7614,11 @@
       <c r="E4" s="30" t="s">
         <v>94</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+      <c r="F4" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A5" s="40" t="s">
         <v>11</v>
       </c>
@@ -7547,7 +7627,7 @@
         <v>4</v>
       </c>
       <c r="C5" s="34" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D5" s="50" t="s">
         <v>12</v>
@@ -7555,8 +7635,11 @@
       <c r="E5" s="30" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="41" t="s">
         <v>14</v>
       </c>
@@ -7565,14 +7648,19 @@
         <v>5</v>
       </c>
       <c r="C6" s="34" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="D6" s="51" t="s">
-        <v>135</v>
-      </c>
-      <c r="E6" s="36"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+        <v>123</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="41" t="s">
         <v>14</v>
       </c>
@@ -7581,14 +7669,19 @@
         <v>6</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>137</v>
-      </c>
-      <c r="E7" s="36"/>
-    </row>
-    <row r="8" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+        <v>125</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="F7" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A8" s="41" t="s">
         <v>14</v>
       </c>
@@ -7597,14 +7690,19 @@
         <v>7</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D8" s="51" t="s">
-        <v>139</v>
-      </c>
-      <c r="E8" s="36"/>
-    </row>
-    <row r="9" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+        <v>127</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="F8" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A9" s="41" t="s">
         <v>14</v>
       </c>
@@ -7613,14 +7711,19 @@
         <v>8</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="D9" s="51" t="s">
-        <v>141</v>
-      </c>
-      <c r="E9" s="36"/>
-    </row>
-    <row r="10" spans="1:5" ht="117" x14ac:dyDescent="0.2">
+        <v>129</v>
+      </c>
+      <c r="E9" s="31" t="s">
+        <v>187</v>
+      </c>
+      <c r="F9" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="117" x14ac:dyDescent="0.2">
       <c r="A10" s="42" t="s">
         <v>14</v>
       </c>
@@ -7634,9 +7737,14 @@
       <c r="D10" s="52" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="36"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E10" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="F10" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="42" t="s">
         <v>14</v>
       </c>
@@ -7645,14 +7753,19 @@
         <v>10</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D11" s="52" t="s">
-        <v>143</v>
-      </c>
-      <c r="E11" s="36"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+        <v>131</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="F11" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="41" t="s">
         <v>14</v>
       </c>
@@ -7661,14 +7774,19 @@
         <v>11</v>
       </c>
       <c r="C12" s="34" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="D12" s="51" t="s">
-        <v>145</v>
-      </c>
-      <c r="E12" s="36"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+        <v>133</v>
+      </c>
+      <c r="E12" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="F12" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="41" t="s">
         <v>14</v>
       </c>
@@ -7677,14 +7795,19 @@
         <v>12</v>
       </c>
       <c r="C13" s="34" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
       <c r="D13" s="51" t="s">
-        <v>147</v>
-      </c>
-      <c r="E13" s="36"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+        <v>135</v>
+      </c>
+      <c r="E13" s="57" t="s">
+        <v>190</v>
+      </c>
+      <c r="F13" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="41" t="s">
         <v>14</v>
       </c>
@@ -7693,14 +7816,19 @@
         <v>13</v>
       </c>
       <c r="C14" s="34" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="D14" s="51" t="s">
-        <v>149</v>
-      </c>
-      <c r="E14" s="36"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+        <v>137</v>
+      </c>
+      <c r="E14" s="57" t="s">
+        <v>191</v>
+      </c>
+      <c r="F14" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="41" t="s">
         <v>14</v>
       </c>
@@ -7709,14 +7837,19 @@
         <v>14</v>
       </c>
       <c r="C15" s="34" t="s">
-        <v>152</v>
+        <v>140</v>
       </c>
       <c r="D15" s="51" t="s">
-        <v>151</v>
-      </c>
-      <c r="E15" s="36"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+        <v>139</v>
+      </c>
+      <c r="E15" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="F15" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="41" t="s">
         <v>14</v>
       </c>
@@ -7725,14 +7858,19 @@
         <v>15</v>
       </c>
       <c r="C16" s="34" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="D16" s="51" t="s">
-        <v>153</v>
-      </c>
-      <c r="E16" s="36"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+        <v>141</v>
+      </c>
+      <c r="E16" s="57" t="s">
+        <v>197</v>
+      </c>
+      <c r="F16" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="41" t="s">
         <v>14</v>
       </c>
@@ -7741,14 +7879,19 @@
         <v>16</v>
       </c>
       <c r="C17" s="34" t="s">
-        <v>156</v>
+        <v>144</v>
       </c>
       <c r="D17" s="51" t="s">
-        <v>155</v>
-      </c>
-      <c r="E17" s="36"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+        <v>143</v>
+      </c>
+      <c r="E17" s="57" t="s">
+        <v>198</v>
+      </c>
+      <c r="F17" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="41" t="s">
         <v>14</v>
       </c>
@@ -7757,14 +7900,19 @@
         <v>17</v>
       </c>
       <c r="C18" s="34" t="s">
-        <v>158</v>
+        <v>146</v>
       </c>
       <c r="D18" s="51" t="s">
-        <v>157</v>
-      </c>
-      <c r="E18" s="36"/>
-    </row>
-    <row r="19" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+        <v>145</v>
+      </c>
+      <c r="E18" s="57" t="s">
+        <v>194</v>
+      </c>
+      <c r="F18" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A19" s="41" t="s">
         <v>14</v>
       </c>
@@ -7773,14 +7921,19 @@
         <v>18</v>
       </c>
       <c r="C19" s="34" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="D19" s="51" t="s">
-        <v>159</v>
-      </c>
-      <c r="E19" s="36"/>
-    </row>
-    <row r="20" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+        <v>147</v>
+      </c>
+      <c r="E19" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="F19" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A20" s="41" t="s">
         <v>14</v>
       </c>
@@ -7789,14 +7942,16 @@
         <v>19</v>
       </c>
       <c r="C20" s="34" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D20" s="51" t="s">
-        <v>161</v>
-      </c>
-      <c r="E20" s="36"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+        <v>149</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="38" t="s">
         <v>3</v>
       </c>
@@ -7805,16 +7960,19 @@
         <v>20</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="D21" s="48" t="s">
         <v>21</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+        <v>98</v>
+      </c>
+      <c r="F21" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="38" t="s">
         <v>3</v>
       </c>
@@ -7829,10 +7987,13 @@
         <v>23</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+        <v>99</v>
+      </c>
+      <c r="F22" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="s">
         <v>3</v>
       </c>
@@ -7847,10 +8008,13 @@
         <v>25</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+      <c r="F23" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="43" t="s">
         <v>3</v>
       </c>
@@ -7865,10 +8029,13 @@
         <v>27</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+        <v>100</v>
+      </c>
+      <c r="F24" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A25" s="43" t="s">
         <v>3</v>
       </c>
@@ -7877,16 +8044,19 @@
         <v>24</v>
       </c>
       <c r="C25" s="35" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D25" s="53" t="s">
         <v>29</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" ht="52" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+      <c r="F25" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A26" s="43" t="s">
         <v>3</v>
       </c>
@@ -7895,16 +8065,16 @@
         <v>25</v>
       </c>
       <c r="C26" s="34" t="s">
-        <v>165</v>
+        <v>153</v>
       </c>
       <c r="D26" s="53" t="s">
         <v>57</v>
       </c>
       <c r="E26" s="33" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="s">
         <v>3</v>
       </c>
@@ -7919,10 +8089,13 @@
         <v>31</v>
       </c>
       <c r="E27" s="30" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+        <v>114</v>
+      </c>
+      <c r="F27" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="38" t="s">
         <v>3</v>
       </c>
@@ -7937,10 +8110,13 @@
         <v>33</v>
       </c>
       <c r="E28" s="32" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+      <c r="F28" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="38" t="s">
         <v>3</v>
       </c>
@@ -7955,10 +8131,13 @@
         <v>35</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+        <v>107</v>
+      </c>
+      <c r="F29" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="38" t="s">
         <v>3</v>
       </c>
@@ -7973,10 +8152,13 @@
         <v>37</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+        <v>102</v>
+      </c>
+      <c r="F30" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="38" t="s">
         <v>3</v>
       </c>
@@ -7991,10 +8173,10 @@
         <v>39</v>
       </c>
       <c r="E31" s="33" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="38" t="s">
         <v>3</v>
       </c>
@@ -8009,10 +8191,13 @@
         <v>41</v>
       </c>
       <c r="E32" s="30" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+      <c r="F32" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33" s="39" t="s">
         <v>8</v>
       </c>
@@ -8021,14 +8206,19 @@
         <v>32</v>
       </c>
       <c r="C33" s="34" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="D33" s="49" t="s">
-        <v>166</v>
-      </c>
-      <c r="E33" s="36"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+        <v>154</v>
+      </c>
+      <c r="E33" s="36" t="s">
+        <v>210</v>
+      </c>
+      <c r="F33" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="39" t="s">
         <v>8</v>
       </c>
@@ -8037,14 +8227,19 @@
         <v>33</v>
       </c>
       <c r="C34" s="34" t="s">
-        <v>169</v>
+        <v>157</v>
       </c>
       <c r="D34" s="49" t="s">
-        <v>168</v>
-      </c>
-      <c r="E34" s="36"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+        <v>156</v>
+      </c>
+      <c r="E34" s="36" t="s">
+        <v>211</v>
+      </c>
+      <c r="F34" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="39" t="s">
         <v>8</v>
       </c>
@@ -8053,14 +8248,19 @@
         <v>34</v>
       </c>
       <c r="C35" s="34" t="s">
-        <v>171</v>
+        <v>159</v>
       </c>
       <c r="D35" s="49" t="s">
-        <v>170</v>
-      </c>
-      <c r="E35" s="36"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+        <v>158</v>
+      </c>
+      <c r="E35" s="30" t="s">
+        <v>112</v>
+      </c>
+      <c r="F35" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="39" t="s">
         <v>8</v>
       </c>
@@ -8069,14 +8269,19 @@
         <v>35</v>
       </c>
       <c r="C36" s="34" t="s">
-        <v>173</v>
+        <v>161</v>
       </c>
       <c r="D36" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="E36" s="36"/>
-    </row>
-    <row r="37" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+        <v>160</v>
+      </c>
+      <c r="E36" s="30" t="s">
+        <v>208</v>
+      </c>
+      <c r="F36" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A37" s="39" t="s">
         <v>8</v>
       </c>
@@ -8085,14 +8290,19 @@
         <v>36</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>174</v>
+        <v>162</v>
       </c>
       <c r="D37" s="49" t="s">
         <v>47</v>
       </c>
-      <c r="E37" s="36"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E37" s="30" t="s">
+        <v>207</v>
+      </c>
+      <c r="F37" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="37" t="s">
         <v>0</v>
       </c>
@@ -8107,10 +8317,13 @@
         <v>49</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+        <v>120</v>
+      </c>
+      <c r="F38" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="39" t="s">
         <v>8</v>
       </c>
@@ -8125,10 +8338,10 @@
         <v>51</v>
       </c>
       <c r="E39" s="33" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="78" x14ac:dyDescent="0.2">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="78" x14ac:dyDescent="0.2">
       <c r="A40" s="42" t="s">
         <v>14</v>
       </c>
@@ -8143,10 +8356,13 @@
         <v>55</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+        <v>111</v>
+      </c>
+      <c r="F40" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A41" s="42" t="s">
         <v>14</v>
       </c>
@@ -8155,14 +8371,19 @@
         <v>40</v>
       </c>
       <c r="C41" s="35" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="D41" s="52" t="s">
         <v>59</v>
       </c>
-      <c r="E41" s="36"/>
-    </row>
-    <row r="42" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+      <c r="E41" s="31" t="s">
+        <v>206</v>
+      </c>
+      <c r="F41" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A42" s="42" t="s">
         <v>14</v>
       </c>
@@ -8171,14 +8392,19 @@
         <v>41</v>
       </c>
       <c r="C42" s="35" t="s">
-        <v>176</v>
+        <v>164</v>
       </c>
       <c r="D42" s="52" t="s">
         <v>61</v>
       </c>
-      <c r="E42" s="36"/>
-    </row>
-    <row r="43" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+      <c r="E42" s="31" t="s">
+        <v>204</v>
+      </c>
+      <c r="F42" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A43" s="42" t="s">
         <v>14</v>
       </c>
@@ -8192,9 +8418,14 @@
       <c r="D43" s="52" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="36"/>
-    </row>
-    <row r="44" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+      <c r="E43" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="F43" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A44" s="37" t="s">
         <v>0</v>
       </c>
@@ -8209,10 +8440,13 @@
         <v>65</v>
       </c>
       <c r="E44" s="30" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="F44" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A45" s="42" t="s">
         <v>14</v>
       </c>
@@ -8226,9 +8460,14 @@
       <c r="D45" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="E45" s="36"/>
-    </row>
-    <row r="46" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+      <c r="E45" s="31" t="s">
+        <v>201</v>
+      </c>
+      <c r="F45" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A46" s="42" t="s">
         <v>14</v>
       </c>
@@ -8242,9 +8481,14 @@
       <c r="D46" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="E46" s="36"/>
-    </row>
-    <row r="47" spans="1:5" ht="52" x14ac:dyDescent="0.2">
+      <c r="E46" s="31" t="s">
+        <v>202</v>
+      </c>
+      <c r="F46" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A47" s="42" t="s">
         <v>14</v>
       </c>
@@ -8253,14 +8497,19 @@
         <v>46</v>
       </c>
       <c r="C47" s="35" t="s">
-        <v>177</v>
+        <v>165</v>
       </c>
       <c r="D47" s="52" t="s">
         <v>71</v>
       </c>
-      <c r="E47" s="36"/>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E47" s="31" t="s">
+        <v>203</v>
+      </c>
+      <c r="F47" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="38" t="s">
         <v>3</v>
       </c>
@@ -8275,10 +8524,13 @@
         <v>73</v>
       </c>
       <c r="E48" s="30" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="F48" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="38" t="s">
         <v>3</v>
       </c>
@@ -8293,10 +8545,13 @@
         <v>75</v>
       </c>
       <c r="E49" s="30" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="50" spans="1:5" ht="52" x14ac:dyDescent="0.2">
+        <v>109</v>
+      </c>
+      <c r="F49" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="52" x14ac:dyDescent="0.2">
       <c r="A50" s="38" t="s">
         <v>3</v>
       </c>
@@ -8305,16 +8560,19 @@
         <v>49</v>
       </c>
       <c r="C50" s="34" t="s">
-        <v>179</v>
+        <v>167</v>
       </c>
       <c r="D50" s="48" t="s">
-        <v>178</v>
+        <v>166</v>
       </c>
       <c r="E50" s="30" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+        <v>173</v>
+      </c>
+      <c r="F50" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="42" t="s">
         <v>14</v>
       </c>
@@ -8323,14 +8581,19 @@
         <v>50</v>
       </c>
       <c r="C51" s="34" t="s">
-        <v>180</v>
+        <v>168</v>
       </c>
       <c r="D51" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="E51" s="36"/>
-    </row>
-    <row r="52" spans="1:5" ht="182" x14ac:dyDescent="0.2">
+      <c r="E51" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F51" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="182" x14ac:dyDescent="0.2">
       <c r="A52" s="42" t="s">
         <v>14</v>
       </c>
@@ -8339,14 +8602,19 @@
         <v>51</v>
       </c>
       <c r="C52" s="34" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D52" s="52" t="s">
         <v>79</v>
       </c>
-      <c r="E52" s="36"/>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E52" s="31" t="s">
+        <v>200</v>
+      </c>
+      <c r="F52" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="42" t="s">
         <v>14</v>
       </c>
@@ -8361,12 +8629,15 @@
         <v>81</v>
       </c>
       <c r="E53" s="30" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" ht="26" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+      <c r="F53" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A54" s="44" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="B54" s="26">
         <f t="shared" si="0"/>
@@ -8379,10 +8650,13 @@
         <v>83</v>
       </c>
       <c r="E54" s="30" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" ht="39" x14ac:dyDescent="0.2">
+        <v>104</v>
+      </c>
+      <c r="F54" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="39" x14ac:dyDescent="0.2">
       <c r="A55" s="37" t="s">
         <v>0</v>
       </c>
@@ -8397,10 +8671,10 @@
         <v>85</v>
       </c>
       <c r="E55" s="30" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="41" t="s">
         <v>14</v>
       </c>
@@ -8414,9 +8688,14 @@
       <c r="D56" s="51" t="s">
         <v>87</v>
       </c>
-      <c r="E56" s="36"/>
-    </row>
-    <row r="57" spans="1:5" ht="91" x14ac:dyDescent="0.2">
+      <c r="E56" s="36" t="s">
+        <v>199</v>
+      </c>
+      <c r="F56" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="91" x14ac:dyDescent="0.2">
       <c r="A57" s="45" t="s">
         <v>3</v>
       </c>
@@ -8425,16 +8704,19 @@
         <v>56</v>
       </c>
       <c r="C57" s="34" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D57" s="55" t="s">
         <v>89</v>
       </c>
       <c r="E57" s="30" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" ht="104" x14ac:dyDescent="0.2">
+        <v>106</v>
+      </c>
+      <c r="F57" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="104" x14ac:dyDescent="0.2">
       <c r="A58" s="45" t="s">
         <v>3</v>
       </c>
@@ -8443,13 +8725,16 @@
         <v>57</v>
       </c>
       <c r="C58" s="34" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D58" s="55" t="s">
         <v>91</v>
       </c>
       <c r="E58" s="30" t="s">
-        <v>118</v>
+        <v>106</v>
+      </c>
+      <c r="F58" s="58" t="s">
+        <v>209</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Latest mods for Seasons
</commit_message>
<xml_diff>
--- a/Doc/XML-SS-Correspondences.xlsx
+++ b/Doc/XML-SS-Correspondences.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="23340" yWindow="1060" windowWidth="24900" windowHeight="27300" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="24340" yWindow="1000" windowWidth="24900" windowHeight="27300" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Movies" sheetId="1" r:id="rId1"/>
     <sheet name="TV (episode)" sheetId="2" r:id="rId2"/>
+    <sheet name="TV (season) " sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="461" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="712" uniqueCount="225">
   <si>
     <t>Avail</t>
   </si>
@@ -751,6 +752,45 @@
   </si>
   <si>
     <t>Avail/Asset/EpisodeMetadata/SeasonMetadata/SeasonContentID</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/SeriesMetadata/TitleInternalAlias</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/SeriesMetadata/TitleDisplayUnlimited</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/SeasonNumber</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/LocalizationOffering</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/SeriesMetadata/NumberOfSeasons</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/SeriesMetadata/AltIdentifier</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/AltIdentifier</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/SeriesMetadata/SeriesContentID</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/SeasonContentID</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/NumberOfEpisodes</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/ReleaseDate</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/TitleInternalAlias</t>
+  </si>
+  <si>
+    <t>Avail/Asset/SeasonMetadata/TitleDisplayUnlimited</t>
   </si>
 </sst>
 </file>
@@ -808,7 +848,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="17">
+  <fills count="22">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -905,6 +945,36 @@
         <bgColor rgb="FFD9EAD3"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF38761D"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFA64D79"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FF85200C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -933,7 +1003,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1098,7 +1168,41 @@
     <xf numFmtId="49" fontId="0" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="18" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="17" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="17" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="21" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -7520,8 +7624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51:E52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7531,7 +7635,7 @@
     <col min="3" max="3" width="61.1640625" customWidth="1"/>
     <col min="4" max="4" width="26.33203125" style="56" customWidth="1"/>
     <col min="5" max="5" width="74" customWidth="1"/>
-    <col min="6" max="6" width="10.83203125" style="58"/>
+    <col min="6" max="6" width="10.83203125" style="59"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -7950,6 +8054,7 @@
       <c r="E20" s="33" t="s">
         <v>113</v>
       </c>
+      <c r="F20" s="58"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="38" t="s">
@@ -8073,6 +8178,7 @@
       <c r="E26" s="33" t="s">
         <v>113</v>
       </c>
+      <c r="F26" s="58"/>
     </row>
     <row r="27" spans="1:6" ht="26" x14ac:dyDescent="0.2">
       <c r="A27" s="38" t="s">
@@ -8175,6 +8281,7 @@
       <c r="E31" s="33" t="s">
         <v>113</v>
       </c>
+      <c r="F31" s="58"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="38" t="s">
@@ -8340,6 +8447,7 @@
       <c r="E39" s="33" t="s">
         <v>113</v>
       </c>
+      <c r="F39" s="58"/>
     </row>
     <row r="40" spans="1:6" ht="78" x14ac:dyDescent="0.2">
       <c r="A40" s="42" t="s">
@@ -8673,6 +8781,7 @@
       <c r="E55" s="30" t="s">
         <v>117</v>
       </c>
+      <c r="F55" s="58"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="41" t="s">
@@ -8736,6 +8845,1169 @@
       <c r="F58" s="58" t="s">
         <v>209</v>
       </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F58"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="F56" sqref="F56"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.1640625" style="46" customWidth="1"/>
+    <col min="2" max="2" width="7.1640625" customWidth="1"/>
+    <col min="3" max="3" width="61.1640625" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="56" customWidth="1"/>
+    <col min="5" max="5" width="74" customWidth="1"/>
+    <col min="6" max="6" width="10.83203125" style="59"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="26">
+        <f>ROW()-1</f>
+        <v>0</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="47" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>110</v>
+      </c>
+      <c r="F1" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="91" x14ac:dyDescent="0.2">
+      <c r="A2" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="26">
+        <f t="shared" ref="B2:B58" si="0">ROW()-1</f>
+        <v>1</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A3" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="C3" s="34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="30" t="s">
+        <v>96</v>
+      </c>
+      <c r="F3" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+      <c r="A4" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="26">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="C4" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="D4" s="49" t="s">
+        <v>9</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>94</v>
+      </c>
+      <c r="F4" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+      <c r="A5" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="26">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="C5" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="50" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>93</v>
+      </c>
+      <c r="F5" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="26">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="C6" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="51" t="s">
+        <v>123</v>
+      </c>
+      <c r="E6" s="31" t="s">
+        <v>212</v>
+      </c>
+      <c r="F6" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="C7" s="34" t="s">
+        <v>126</v>
+      </c>
+      <c r="D7" s="51" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="F7" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A8" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="26">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="34" t="s">
+        <v>128</v>
+      </c>
+      <c r="D8" s="51" t="s">
+        <v>127</v>
+      </c>
+      <c r="E8" s="31" t="s">
+        <v>214</v>
+      </c>
+      <c r="F8" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+      <c r="A9" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="26">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="C9" s="34" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="61" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="60"/>
+      <c r="F9" s="69"/>
+    </row>
+    <row r="10" spans="1:6" ht="117" x14ac:dyDescent="0.2">
+      <c r="A10" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="26">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C10" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="52" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>215</v>
+      </c>
+      <c r="F10" s="58"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="26">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>132</v>
+      </c>
+      <c r="D11" s="62" t="s">
+        <v>131</v>
+      </c>
+      <c r="E11" s="60"/>
+      <c r="F11" s="69"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="26">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>134</v>
+      </c>
+      <c r="D12" s="61" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" s="60"/>
+      <c r="F12" s="69"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B13" s="26">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="C13" s="34" t="s">
+        <v>136</v>
+      </c>
+      <c r="D13" s="51" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" s="57" t="s">
+        <v>223</v>
+      </c>
+      <c r="F13" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="26">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C14" s="34" t="s">
+        <v>138</v>
+      </c>
+      <c r="D14" s="51" t="s">
+        <v>137</v>
+      </c>
+      <c r="E14" s="57" t="s">
+        <v>224</v>
+      </c>
+      <c r="F14" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="26">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="C15" s="34" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" s="51" t="s">
+        <v>139</v>
+      </c>
+      <c r="E15" s="57" t="s">
+        <v>221</v>
+      </c>
+      <c r="F15" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="26">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C16" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="D16" s="51" t="s">
+        <v>141</v>
+      </c>
+      <c r="E16" s="57" t="s">
+        <v>216</v>
+      </c>
+      <c r="F16" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="26">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="C17" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="D17" s="51" t="s">
+        <v>143</v>
+      </c>
+      <c r="E17" s="57" t="s">
+        <v>217</v>
+      </c>
+      <c r="F17" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18" s="26">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C18" s="34" t="s">
+        <v>146</v>
+      </c>
+      <c r="D18" s="51" t="s">
+        <v>145</v>
+      </c>
+      <c r="E18" s="57" t="s">
+        <v>218</v>
+      </c>
+      <c r="F18" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A19" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B19" s="26">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="C19" s="34" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="61" t="s">
+        <v>147</v>
+      </c>
+      <c r="E19" s="60"/>
+      <c r="F19" s="69"/>
+    </row>
+    <row r="20" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+      <c r="A20" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B20" s="26">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C20" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" s="51" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="F20" s="70"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="26">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="D21" s="48" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="30" t="s">
+        <v>98</v>
+      </c>
+      <c r="F21" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="26">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="48" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>99</v>
+      </c>
+      <c r="F22" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A23" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="26">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="D23" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="30" t="s">
+        <v>103</v>
+      </c>
+      <c r="F23" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="26">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="53" t="s">
+        <v>27</v>
+      </c>
+      <c r="E24" s="30" t="s">
+        <v>100</v>
+      </c>
+      <c r="F24" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A25" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="26">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="C25" s="35" t="s">
+        <v>152</v>
+      </c>
+      <c r="D25" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="30" t="s">
+        <v>101</v>
+      </c>
+      <c r="F25" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="52" x14ac:dyDescent="0.2">
+      <c r="A26" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="D26" s="53" t="s">
+        <v>57</v>
+      </c>
+      <c r="E26" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="F26" s="70"/>
+    </row>
+    <row r="27" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A27" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="26">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="C27" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="48" t="s">
+        <v>31</v>
+      </c>
+      <c r="E27" s="30" t="s">
+        <v>114</v>
+      </c>
+      <c r="F27" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28" s="26">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C28" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="D28" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>115</v>
+      </c>
+      <c r="F28" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29" s="26">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>36</v>
+      </c>
+      <c r="D29" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>107</v>
+      </c>
+      <c r="F29" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A30" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30" s="26">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="C30" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="D30" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="30" t="s">
+        <v>102</v>
+      </c>
+      <c r="F30" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A31" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31" s="26">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="C31" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="E31" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="70"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32" s="26">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C32" s="34" t="s">
+        <v>42</v>
+      </c>
+      <c r="D32" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F32" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" s="26">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="C33" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="D33" s="49" t="s">
+        <v>154</v>
+      </c>
+      <c r="E33" s="36" t="s">
+        <v>219</v>
+      </c>
+      <c r="F33" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="26">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="C34" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="D34" s="49" t="s">
+        <v>156</v>
+      </c>
+      <c r="E34" s="36" t="s">
+        <v>220</v>
+      </c>
+      <c r="F34" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" s="26">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="C35" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="D35" s="63" t="s">
+        <v>158</v>
+      </c>
+      <c r="E35" s="64"/>
+      <c r="F35" s="69"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" s="26">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C36" s="34" t="s">
+        <v>161</v>
+      </c>
+      <c r="D36" s="63" t="s">
+        <v>160</v>
+      </c>
+      <c r="E36" s="64"/>
+      <c r="F36" s="69"/>
+    </row>
+    <row r="37" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A37" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="26">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="C37" s="34" t="s">
+        <v>162</v>
+      </c>
+      <c r="D37" s="63" t="s">
+        <v>47</v>
+      </c>
+      <c r="E37" s="64"/>
+      <c r="F37" s="69"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38" s="26">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="C38" s="34" t="s">
+        <v>50</v>
+      </c>
+      <c r="D38" s="47" t="s">
+        <v>49</v>
+      </c>
+      <c r="E38" s="30" t="s">
+        <v>120</v>
+      </c>
+      <c r="F38" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="39" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="26">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="C39" s="34" t="s">
+        <v>52</v>
+      </c>
+      <c r="D39" s="49" t="s">
+        <v>51</v>
+      </c>
+      <c r="E39" s="33" t="s">
+        <v>113</v>
+      </c>
+      <c r="F39" s="70"/>
+    </row>
+    <row r="40" spans="1:6" ht="78" x14ac:dyDescent="0.2">
+      <c r="A40" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B40" s="26">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C40" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D40" s="52" t="s">
+        <v>55</v>
+      </c>
+      <c r="E40" s="30" t="s">
+        <v>111</v>
+      </c>
+      <c r="F40" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A41" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B41" s="26">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>163</v>
+      </c>
+      <c r="D41" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="E41" s="31" t="s">
+        <v>222</v>
+      </c>
+      <c r="F41" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+      <c r="A42" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="26">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>164</v>
+      </c>
+      <c r="D42" s="62" t="s">
+        <v>61</v>
+      </c>
+      <c r="E42" s="60"/>
+      <c r="F42" s="69"/>
+    </row>
+    <row r="43" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+      <c r="A43" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43" s="26">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="C43" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="D43" s="62" t="s">
+        <v>63</v>
+      </c>
+      <c r="E43" s="60"/>
+      <c r="F43" s="69"/>
+    </row>
+    <row r="44" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+      <c r="A44" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44" s="26">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="C44" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D44" s="47" t="s">
+        <v>65</v>
+      </c>
+      <c r="E44" s="30" t="s">
+        <v>108</v>
+      </c>
+      <c r="F44" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+      <c r="A45" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="26">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="C45" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D45" s="68" t="s">
+        <v>67</v>
+      </c>
+      <c r="E45" s="60"/>
+      <c r="F45" s="69"/>
+    </row>
+    <row r="46" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A46" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B46" s="26">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C46" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="D46" s="68" t="s">
+        <v>69</v>
+      </c>
+      <c r="E46" s="60"/>
+      <c r="F46" s="69"/>
+    </row>
+    <row r="47" spans="1:6" ht="52" x14ac:dyDescent="0.2">
+      <c r="A47" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B47" s="26">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="C47" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="D47" s="68" t="s">
+        <v>71</v>
+      </c>
+      <c r="E47" s="60"/>
+      <c r="F47" s="69"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="26">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="C48" s="34" t="s">
+        <v>74</v>
+      </c>
+      <c r="D48" s="48" t="s">
+        <v>73</v>
+      </c>
+      <c r="E48" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="F48" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="26">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="C49" s="34" t="s">
+        <v>76</v>
+      </c>
+      <c r="D49" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="E49" s="30" t="s">
+        <v>109</v>
+      </c>
+      <c r="F49" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="52" x14ac:dyDescent="0.2">
+      <c r="A50" s="38" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="26">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="C50" s="34" t="s">
+        <v>167</v>
+      </c>
+      <c r="D50" s="48" t="s">
+        <v>166</v>
+      </c>
+      <c r="E50" s="30" t="s">
+        <v>173</v>
+      </c>
+      <c r="F50" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B51" s="26">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="C51" s="34" t="s">
+        <v>168</v>
+      </c>
+      <c r="D51" s="62" t="s">
+        <v>77</v>
+      </c>
+      <c r="E51" s="65"/>
+      <c r="F51" s="69"/>
+    </row>
+    <row r="52" spans="1:6" ht="182" x14ac:dyDescent="0.2">
+      <c r="A52" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="26">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="C52" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="D52" s="62" t="s">
+        <v>79</v>
+      </c>
+      <c r="E52" s="60"/>
+      <c r="F52" s="69"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="B53" s="26">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="C53" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="D53" s="52" t="s">
+        <v>81</v>
+      </c>
+      <c r="E53" s="30" t="s">
+        <v>116</v>
+      </c>
+      <c r="F53" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="26" x14ac:dyDescent="0.2">
+      <c r="A54" s="44" t="s">
+        <v>170</v>
+      </c>
+      <c r="B54" s="26">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="C54" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="D54" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="E54" s="30" t="s">
+        <v>104</v>
+      </c>
+      <c r="F54" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="39" x14ac:dyDescent="0.2">
+      <c r="A55" s="37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B55" s="26">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="C55" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="D55" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="E55" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="F55" s="58" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A56" s="41" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56" s="26">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="C56" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="D56" s="61" t="s">
+        <v>87</v>
+      </c>
+      <c r="E56" s="66"/>
+      <c r="F56" s="69"/>
+    </row>
+    <row r="57" spans="1:6" ht="91" x14ac:dyDescent="0.2">
+      <c r="A57" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="26">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="C57" s="34" t="s">
+        <v>171</v>
+      </c>
+      <c r="D57" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="E57" s="64"/>
+      <c r="F57" s="69"/>
+    </row>
+    <row r="58" spans="1:6" ht="104" x14ac:dyDescent="0.2">
+      <c r="A58" s="45" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="26">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="C58" s="34" t="s">
+        <v>172</v>
+      </c>
+      <c r="D58" s="67" t="s">
+        <v>91</v>
+      </c>
+      <c r="E58" s="64"/>
+      <c r="F58" s="69"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Cleaned up for first public distribution.
</commit_message>
<xml_diff>
--- a/Doc/XML-SS-Correspondences.xlsx
+++ b/Doc/XML-SS-Correspondences.xlsx
@@ -800,7 +800,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -846,6 +846,22 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="22">
@@ -1000,8 +1016,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1206,7 +1224,9 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -8855,8 +8875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>